<commit_message>
Adição do Planejamento Semanal 24/08
</commit_message>
<xml_diff>
--- a/Documentos/Planejamento_semana3_Agosto_GOVagas.xlsx
+++ b/Documentos/Planejamento_semana3_Agosto_GOVagas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Documents\Backupe\Documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26B90D28-4ADB-4868-9C07-2E62AB366BB4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B65AEDDC-FB6E-43EC-9D1E-C17AF3F357B5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="56">
   <si>
     <t>PLANEJAMENTO SEMANAL - CONTROLE CLASSROOM</t>
   </si>
@@ -121,12 +121,6 @@
     <t>VISUALIZAR PERFIL PSICOLÓGICO (MOBILE)</t>
   </si>
   <si>
-    <t>EDITAR PERFIL PSICOLÓGICO (WEB)</t>
-  </si>
-  <si>
-    <t>EDITAR PERFIL PSICOLÓGICO (MOBILE)</t>
-  </si>
-  <si>
     <t>TELAS DE SUCESSO (WEB)</t>
   </si>
   <si>
@@ -167,6 +161,33 @@
   </si>
   <si>
     <t>TELA SOBRE (MOBILE)</t>
+  </si>
+  <si>
+    <t>AUTO-CONTRASTE</t>
+  </si>
+  <si>
+    <t>TELA ESCURA</t>
+  </si>
+  <si>
+    <t>ACESSIBILIDADE AUDIOVISUAL</t>
+  </si>
+  <si>
+    <t>DAVI</t>
+  </si>
+  <si>
+    <t>GABI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RENAN </t>
+  </si>
+  <si>
+    <t>FÁBIO</t>
+  </si>
+  <si>
+    <t>TELA DE CONFIG DO ALUNO (WEB)</t>
+  </si>
+  <si>
+    <t>TELA DE CONFIG DO ALUNO (MOBILE)</t>
   </si>
 </sst>
 </file>
@@ -594,10 +615,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:T31"/>
+  <dimension ref="A1:T39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -800,7 +821,9 @@
       <c r="E6" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="F6" s="11"/>
+      <c r="F6" s="11" t="s">
+        <v>21</v>
+      </c>
       <c r="G6" s="11"/>
       <c r="H6" s="3"/>
       <c r="I6" s="12"/>
@@ -830,7 +853,9 @@
       <c r="E7" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="F7" s="11"/>
+      <c r="F7" s="11" t="s">
+        <v>21</v>
+      </c>
       <c r="G7" s="11"/>
       <c r="H7" s="3"/>
       <c r="I7" s="12"/>
@@ -860,7 +885,9 @@
       <c r="E8" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="F8" s="11"/>
+      <c r="F8" s="11" t="s">
+        <v>51</v>
+      </c>
       <c r="G8" s="11"/>
       <c r="H8" s="3"/>
       <c r="I8" s="12"/>
@@ -890,7 +917,9 @@
       <c r="E9" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="F9" s="11"/>
+      <c r="F9" s="11" t="s">
+        <v>51</v>
+      </c>
       <c r="G9" s="11"/>
       <c r="H9" s="3"/>
       <c r="I9" s="12"/>
@@ -910,13 +939,17 @@
       <c r="A10" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="B10" s="11"/>
+      <c r="B10" s="11" t="s">
+        <v>50</v>
+      </c>
       <c r="C10" s="11"/>
       <c r="D10" s="3"/>
       <c r="E10" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="F10" s="11"/>
+      <c r="F10" s="11" t="s">
+        <v>51</v>
+      </c>
       <c r="G10" s="11"/>
       <c r="H10" s="3"/>
       <c r="I10" s="11"/>
@@ -936,13 +969,17 @@
       <c r="A11" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="B11" s="11"/>
+      <c r="B11" s="11" t="s">
+        <v>50</v>
+      </c>
       <c r="C11" s="11"/>
       <c r="D11" s="3"/>
       <c r="E11" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="F11" s="11"/>
+        <v>34</v>
+      </c>
+      <c r="F11" s="11" t="s">
+        <v>51</v>
+      </c>
       <c r="G11" s="11"/>
       <c r="H11" s="3"/>
       <c r="I11" s="11"/>
@@ -960,15 +997,21 @@
     </row>
     <row r="12" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A12" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="B12" s="11"/>
-      <c r="C12" s="11"/>
+        <v>40</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="C12" s="12" t="s">
+        <v>26</v>
+      </c>
       <c r="D12" s="3"/>
-      <c r="E12" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="F12" s="11"/>
+      <c r="E12" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="F12" s="11" t="s">
+        <v>52</v>
+      </c>
       <c r="G12" s="11"/>
       <c r="H12" s="3"/>
       <c r="I12" s="11"/>
@@ -988,13 +1031,19 @@
       <c r="A13" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="B13" s="11"/>
-      <c r="C13" s="11"/>
+      <c r="B13" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>26</v>
+      </c>
       <c r="D13" s="3"/>
-      <c r="E13" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="F13" s="11"/>
+      <c r="E13" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="F13" s="11" t="s">
+        <v>52</v>
+      </c>
       <c r="G13" s="11"/>
       <c r="H13" s="3"/>
       <c r="I13" s="11"/>
@@ -1012,15 +1061,19 @@
     </row>
     <row r="14" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A14" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="B14" s="11"/>
+        <v>36</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>50</v>
+      </c>
       <c r="C14" s="11"/>
       <c r="D14" s="3"/>
       <c r="E14" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="F14" s="11"/>
+      <c r="F14" s="11" t="s">
+        <v>50</v>
+      </c>
       <c r="G14" s="11"/>
       <c r="H14" s="3"/>
       <c r="I14" s="11"/>
@@ -1038,15 +1091,19 @@
     </row>
     <row r="15" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A15" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="B15" s="11"/>
+        <v>37</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>50</v>
+      </c>
       <c r="C15" s="11"/>
       <c r="D15" s="3"/>
       <c r="E15" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="F15" s="11"/>
+      <c r="F15" s="11" t="s">
+        <v>50</v>
+      </c>
       <c r="G15" s="11"/>
       <c r="H15" s="3"/>
       <c r="I15" s="11"/>
@@ -1064,15 +1121,19 @@
     </row>
     <row r="16" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="B16" s="11"/>
+        <v>38</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>50</v>
+      </c>
       <c r="C16" s="11"/>
       <c r="D16" s="3"/>
       <c r="E16" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="F16" s="11"/>
+        <v>47</v>
+      </c>
+      <c r="F16" s="11" t="s">
+        <v>53</v>
+      </c>
       <c r="G16" s="11"/>
       <c r="H16" s="3"/>
       <c r="I16" s="11"/>
@@ -1090,15 +1151,19 @@
     </row>
     <row r="17" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="B17" s="11"/>
+        <v>39</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>50</v>
+      </c>
       <c r="C17" s="11"/>
       <c r="D17" s="3"/>
       <c r="E17" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="F17" s="11"/>
+        <v>48</v>
+      </c>
+      <c r="F17" s="11" t="s">
+        <v>53</v>
+      </c>
       <c r="G17" s="11"/>
       <c r="H17" s="3"/>
       <c r="I17" s="11"/>
@@ -1116,13 +1181,21 @@
     </row>
     <row r="18" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="B18" s="7"/>
-      <c r="C18" s="7"/>
+        <v>45</v>
+      </c>
+      <c r="B18" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C18" s="12" t="s">
+        <v>26</v>
+      </c>
       <c r="D18" s="3"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="7"/>
+      <c r="E18" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="F18" s="11" t="s">
+        <v>53</v>
+      </c>
       <c r="G18" s="7"/>
       <c r="H18" s="3"/>
       <c r="I18" s="7"/>
@@ -1140,13 +1213,17 @@
     </row>
     <row r="19" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="B19" s="11"/>
-      <c r="C19" s="11"/>
+        <v>46</v>
+      </c>
+      <c r="B19" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C19" s="12" t="s">
+        <v>26</v>
+      </c>
       <c r="D19" s="3"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="7"/>
+      <c r="E19" s="11"/>
+      <c r="F19" s="11"/>
       <c r="G19" s="7"/>
       <c r="H19" s="3"/>
       <c r="I19" s="7"/>
@@ -1163,58 +1240,246 @@
       <c r="T19" s="3"/>
     </row>
     <row r="20" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B20" s="11"/>
-      <c r="C20" s="8"/>
-      <c r="D20" s="8"/>
-      <c r="E20" s="8"/>
-      <c r="F20" s="8"/>
-      <c r="G20" s="8"/>
-      <c r="H20" s="8"/>
-      <c r="I20" s="8"/>
-      <c r="J20" s="9"/>
-      <c r="K20" s="9" t="s">
+      <c r="A20" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="B20" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="C20" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="D20" s="3"/>
+      <c r="E20" s="11"/>
+      <c r="F20" s="11"/>
+      <c r="G20" s="7"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="7"/>
+      <c r="J20" s="7"/>
+      <c r="K20" s="7"/>
+      <c r="L20" s="3"/>
+      <c r="M20" s="7"/>
+      <c r="N20" s="7"/>
+      <c r="O20" s="7"/>
+      <c r="P20" s="3"/>
+      <c r="Q20" s="7"/>
+      <c r="R20" s="7"/>
+      <c r="S20" s="7"/>
+      <c r="T20" s="3"/>
+    </row>
+    <row r="21" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="B21" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="C21" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="D21" s="3"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="7"/>
+      <c r="G21" s="7"/>
+      <c r="H21" s="3"/>
+      <c r="I21" s="7"/>
+      <c r="J21" s="7"/>
+      <c r="K21" s="7"/>
+      <c r="L21" s="3"/>
+      <c r="M21" s="7"/>
+      <c r="N21" s="7"/>
+      <c r="O21" s="7"/>
+      <c r="P21" s="3"/>
+      <c r="Q21" s="7"/>
+      <c r="R21" s="7"/>
+      <c r="S21" s="7"/>
+      <c r="T21" s="3"/>
+    </row>
+    <row r="22" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="11"/>
+      <c r="B22" s="7"/>
+      <c r="C22" s="7"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="7"/>
+      <c r="F22" s="7"/>
+      <c r="G22" s="7"/>
+      <c r="H22" s="3"/>
+      <c r="I22" s="7"/>
+      <c r="J22" s="7"/>
+      <c r="K22" s="7"/>
+      <c r="L22" s="3"/>
+      <c r="M22" s="7"/>
+      <c r="N22" s="7"/>
+      <c r="O22" s="7"/>
+      <c r="P22" s="3"/>
+      <c r="Q22" s="7"/>
+      <c r="R22" s="7"/>
+      <c r="S22" s="7"/>
+      <c r="T22" s="3"/>
+    </row>
+    <row r="23" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="11"/>
+      <c r="B23" s="7"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="7"/>
+      <c r="G23" s="7"/>
+      <c r="H23" s="3"/>
+      <c r="I23" s="7"/>
+      <c r="J23" s="7"/>
+      <c r="K23" s="7"/>
+      <c r="L23" s="3"/>
+      <c r="M23" s="7"/>
+      <c r="N23" s="7"/>
+      <c r="O23" s="7"/>
+      <c r="P23" s="3"/>
+      <c r="Q23" s="7"/>
+      <c r="R23" s="7"/>
+      <c r="S23" s="7"/>
+      <c r="T23" s="3"/>
+    </row>
+    <row r="24" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="11"/>
+      <c r="B24" s="7"/>
+      <c r="C24" s="7"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="7"/>
+      <c r="F24" s="7"/>
+      <c r="G24" s="7"/>
+      <c r="H24" s="3"/>
+      <c r="I24" s="7"/>
+      <c r="J24" s="7"/>
+      <c r="K24" s="7"/>
+      <c r="L24" s="3"/>
+      <c r="M24" s="7"/>
+      <c r="N24" s="7"/>
+      <c r="O24" s="7"/>
+      <c r="P24" s="3"/>
+      <c r="Q24" s="7"/>
+      <c r="R24" s="7"/>
+      <c r="S24" s="7"/>
+      <c r="T24" s="3"/>
+    </row>
+    <row r="25" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="11"/>
+      <c r="B25" s="7"/>
+      <c r="C25" s="7"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="7"/>
+      <c r="F25" s="7"/>
+      <c r="G25" s="7"/>
+      <c r="H25" s="3"/>
+      <c r="I25" s="7"/>
+      <c r="J25" s="7"/>
+      <c r="K25" s="7"/>
+      <c r="L25" s="3"/>
+      <c r="M25" s="7"/>
+      <c r="N25" s="7"/>
+      <c r="O25" s="7"/>
+      <c r="P25" s="3"/>
+      <c r="Q25" s="7"/>
+      <c r="R25" s="7"/>
+      <c r="S25" s="7"/>
+      <c r="T25" s="3"/>
+    </row>
+    <row r="26" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="11"/>
+      <c r="B26" s="7"/>
+      <c r="C26" s="7"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="7"/>
+      <c r="F26" s="7"/>
+      <c r="G26" s="7"/>
+      <c r="H26" s="3"/>
+      <c r="I26" s="7"/>
+      <c r="J26" s="7"/>
+      <c r="K26" s="7"/>
+      <c r="L26" s="3"/>
+      <c r="M26" s="7"/>
+      <c r="N26" s="7"/>
+      <c r="O26" s="7"/>
+      <c r="P26" s="3"/>
+      <c r="Q26" s="7"/>
+      <c r="R26" s="7"/>
+      <c r="S26" s="7"/>
+      <c r="T26" s="3"/>
+    </row>
+    <row r="27" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="11"/>
+      <c r="B27" s="11"/>
+      <c r="C27" s="11"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="7"/>
+      <c r="F27" s="7"/>
+      <c r="G27" s="7"/>
+      <c r="H27" s="3"/>
+      <c r="I27" s="7"/>
+      <c r="J27" s="7"/>
+      <c r="K27" s="7"/>
+      <c r="L27" s="3"/>
+      <c r="M27" s="7"/>
+      <c r="N27" s="7"/>
+      <c r="O27" s="7"/>
+      <c r="P27" s="3"/>
+      <c r="Q27" s="7"/>
+      <c r="R27" s="7"/>
+      <c r="S27" s="7"/>
+      <c r="T27" s="3"/>
+    </row>
+    <row r="28" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B28" s="11"/>
+      <c r="C28" s="8"/>
+      <c r="D28" s="8"/>
+      <c r="E28" s="8"/>
+      <c r="F28" s="8"/>
+      <c r="G28" s="8"/>
+      <c r="H28" s="8"/>
+      <c r="I28" s="8"/>
+      <c r="J28" s="9"/>
+      <c r="K28" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="L20" s="9"/>
-      <c r="M20" s="9"/>
-      <c r="N20" s="9"/>
-      <c r="O20" s="9"/>
-      <c r="P20" s="9"/>
-      <c r="Q20" s="9"/>
-      <c r="R20" s="9"/>
-      <c r="S20" s="9"/>
-      <c r="T20" s="9"/>
-    </row>
-    <row r="22" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="10" t="s">
+      <c r="L28" s="9"/>
+      <c r="M28" s="9"/>
+      <c r="N28" s="9"/>
+      <c r="O28" s="9"/>
+      <c r="P28" s="9"/>
+      <c r="Q28" s="9"/>
+      <c r="R28" s="9"/>
+      <c r="S28" s="9"/>
+      <c r="T28" s="9"/>
+    </row>
+    <row r="30" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="10" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="23" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="10" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="25" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="10" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="27" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="10" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="29" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="10" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="30" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="10"/>
     </row>
     <row r="31" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="10"/>
+    </row>
+    <row r="39" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="10" t="s">
         <v>20</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Correções Doc Planejamento 24/08
</commit_message>
<xml_diff>
--- a/Documentos/Planejamento_semana3_Agosto_GOVagas.xlsx
+++ b/Documentos/Planejamento_semana3_Agosto_GOVagas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Documents\Backupe\Documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB1F5E6F-6347-470F-884D-B6C61C3B9EB8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E017EC2D-AC4F-4CBD-8B3E-65A7FB22C245}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="57">
   <si>
     <t>PLANEJAMENTO SEMANAL - CONTROLE CLASSROOM</t>
   </si>
@@ -188,6 +188,9 @@
   </si>
   <si>
     <t>TELA DE CONFIG DO ALUNO (MOBILE)</t>
+  </si>
+  <si>
+    <t>FÁBIO/RENAN</t>
   </si>
 </sst>
 </file>
@@ -618,7 +621,7 @@
   <dimension ref="A1:T39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1132,7 +1135,7 @@
         <v>47</v>
       </c>
       <c r="F16" s="11" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="G16" s="11"/>
       <c r="H16" s="3"/>
@@ -1162,7 +1165,7 @@
         <v>48</v>
       </c>
       <c r="F17" s="11" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="G17" s="11"/>
       <c r="H17" s="3"/>
@@ -1194,7 +1197,7 @@
         <v>49</v>
       </c>
       <c r="F18" s="11" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="G18" s="7"/>
       <c r="H18" s="3"/>

</xml_diff>